<commit_message>
g2.3 - reestruturação para evitar erro de referência
</commit_message>
<xml_diff>
--- a/Data/g2.3.xlsx
+++ b/Data/g2.3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,22 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Quantidade 2023/2010</t>
+          <t>Categoria</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Valor 2023/2010</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Quantidade 2023/2022</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Valor 2023/2022</t>
+          <t>Valor</t>
         </is>
       </c>
     </row>
@@ -466,17 +456,13 @@
           <t>Abacaxi*</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Quantidade 2023/2010</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>47.83246265236917</v>
-      </c>
-      <c r="C2" t="n">
-        <v>33.02074801780581</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1.850097872071731</v>
-      </c>
-      <c r="E2" t="n">
-        <v>38.13303529810645</v>
       </c>
     </row>
     <row r="3">
@@ -485,17 +471,13 @@
           <t>Batata-doce</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Quantidade 2023/2010</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>78.77826365187714</v>
-      </c>
-      <c r="C3" t="n">
-        <v>130.9992725211956</v>
-      </c>
-      <c r="D3" t="n">
-        <v>3.885901984784865</v>
-      </c>
-      <c r="E3" t="n">
-        <v>46.60236769419782</v>
       </c>
     </row>
     <row r="4">
@@ -504,17 +486,13 @@
           <t>Cana-de-açúcar</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Quantidade 2023/2010</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>-17.32238242110792</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-52.79088281755887</v>
-      </c>
-      <c r="D4" t="n">
-        <v>13.4046328339834</v>
-      </c>
-      <c r="E4" t="n">
-        <v>32.00053638077491</v>
       </c>
     </row>
     <row r="5">
@@ -523,17 +501,13 @@
           <t>Mandioca</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Quantidade 2023/2010</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>-65.77736113400363</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-37.88225480837426</v>
-      </c>
-      <c r="D5" t="n">
-        <v>5.811568352656389</v>
-      </c>
-      <c r="E5" t="n">
-        <v>21.47332385208742</v>
       </c>
     </row>
     <row r="6">
@@ -542,17 +516,13 @@
           <t>Melancia</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Quantidade 2023/2010</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>-77.78776978417267</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-63.85171938721052</v>
-      </c>
-      <c r="D6" t="n">
-        <v>12.3237835379718</v>
-      </c>
-      <c r="E6" t="n">
-        <v>64.6428865948227</v>
       </c>
     </row>
     <row r="7">
@@ -561,16 +531,282 @@
           <t>Tomate</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Quantidade 2023/2010</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>18.66985437948272</v>
       </c>
-      <c r="C7" t="n">
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Abacaxi*</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Valor 2023/2010</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>33.02074801780581</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Batata-doce</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Valor 2023/2010</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>130.9992725211956</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Cana-de-açúcar</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Valor 2023/2010</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>-52.79088281755887</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Mandioca</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Valor 2023/2010</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>-37.88225480837426</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Melancia</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Valor 2023/2010</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>-63.85171938721052</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Tomate</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Valor 2023/2010</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
         <v>18.74749397486748</v>
       </c>
-      <c r="D7" t="n">
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Abacaxi*</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Quantidade 2023/2022</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1.850097872071731</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Batata-doce</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Quantidade 2023/2022</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>3.885901984784865</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Cana-de-açúcar</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Quantidade 2023/2022</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>13.4046328339834</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mandioca</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Quantidade 2023/2022</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>5.811568352656389</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Melancia</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Quantidade 2023/2022</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>12.3237835379718</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Tomate</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Quantidade 2023/2022</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
         <v>-36.95150115473441</v>
       </c>
-      <c r="E7" t="n">
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Abacaxi*</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Valor 2023/2022</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>38.13303529810645</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Batata-doce</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Valor 2023/2022</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>46.60236769419782</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Cana-de-açúcar</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Valor 2023/2022</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>32.00053638077491</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Mandioca</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Valor 2023/2022</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>21.47332385208742</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Melancia</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Valor 2023/2022</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>64.6428865948227</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Tomate</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Valor 2023/2022</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
         <v>-30.40227332240353</v>
       </c>
     </row>

</xml_diff>

<commit_message>
g2.3 - ajuste no nome da coluna
</commit_message>
<xml_diff>
--- a/Data/g2.3.xlsx
+++ b/Data/g2.3.xlsx
@@ -458,11 +458,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Quantidade 2023/2010</t>
+          <t>Quantidade (atual/dez anos antes)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>47.83246265236917</v>
+        <v>69.07756813417191</v>
       </c>
     </row>
     <row r="3">
@@ -473,11 +473,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Quantidade 2023/2010</t>
+          <t>Quantidade (atual/dez anos antes)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>78.77826365187714</v>
+        <v>51.02146541432979</v>
       </c>
     </row>
     <row r="4">
@@ -488,11 +488,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Quantidade 2023/2010</t>
+          <t>Quantidade (atual/dez anos antes)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-17.32238242110792</v>
+        <v>-19.79246840347153</v>
       </c>
     </row>
     <row r="5">
@@ -503,11 +503,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Quantidade 2023/2010</t>
+          <t>Quantidade (atual/dez anos antes)</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-65.77736113400363</v>
+        <v>-61.70297632359825</v>
       </c>
     </row>
     <row r="6">
@@ -518,11 +518,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Quantidade 2023/2010</t>
+          <t>Quantidade (atual/dez anos antes)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-77.78776978417267</v>
+        <v>-70.15466408893185</v>
       </c>
     </row>
     <row r="7">
@@ -533,11 +533,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Quantidade 2023/2010</t>
+          <t>Quantidade (atual/dez anos antes)</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>18.66985437948272</v>
+        <v>110.3235747303544</v>
       </c>
     </row>
     <row r="8">
@@ -548,11 +548,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Valor 2023/2010</t>
+          <t>Valor (atual/dez anos antes)</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>33.02074801780581</v>
+        <v>39.20704066561322</v>
       </c>
     </row>
     <row r="9">
@@ -563,11 +563,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Valor 2023/2010</t>
+          <t>Valor (atual/dez anos antes)</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>130.9992725211956</v>
+        <v>111.3766687945756</v>
       </c>
     </row>
     <row r="10">
@@ -578,11 +578,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Valor 2023/2010</t>
+          <t>Valor (atual/dez anos antes)</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-52.79088281755887</v>
+        <v>-38.80258191846784</v>
       </c>
     </row>
     <row r="11">
@@ -593,11 +593,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Valor 2023/2010</t>
+          <t>Valor (atual/dez anos antes)</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-37.88225480837426</v>
+        <v>-75.00701801464335</v>
       </c>
     </row>
     <row r="12">
@@ -608,11 +608,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Valor 2023/2010</t>
+          <t>Valor (atual/dez anos antes)</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-63.85171938721052</v>
+        <v>-66.55807726662741</v>
       </c>
     </row>
     <row r="13">
@@ -623,11 +623,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Valor 2023/2010</t>
+          <t>Valor (atual/dez anos antes)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>18.74749397486748</v>
+        <v>33.87882696012225</v>
       </c>
     </row>
     <row r="14">
@@ -638,7 +638,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Quantidade 2023/2022</t>
+          <t>Quantidade (atual/ano anterior)</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -653,7 +653,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Quantidade 2023/2022</t>
+          <t>Quantidade (atual/ano anterior)</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -668,7 +668,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Quantidade 2023/2022</t>
+          <t>Quantidade (atual/ano anterior)</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -683,7 +683,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Quantidade 2023/2022</t>
+          <t>Quantidade (atual/ano anterior)</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -698,7 +698,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Quantidade 2023/2022</t>
+          <t>Quantidade (atual/ano anterior)</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -713,7 +713,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Quantidade 2023/2022</t>
+          <t>Quantidade (atual/ano anterior)</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -728,7 +728,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Valor 2023/2022</t>
+          <t>Valor (atual/ano anterior)</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -743,7 +743,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Valor 2023/2022</t>
+          <t>Valor (atual/ano anterior)</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -758,7 +758,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Valor 2023/2022</t>
+          <t>Valor (atual/ano anterior)</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -773,7 +773,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Valor 2023/2022</t>
+          <t>Valor (atual/ano anterior)</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -788,7 +788,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Valor 2023/2022</t>
+          <t>Valor (atual/ano anterior)</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -803,7 +803,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Valor 2023/2022</t>
+          <t>Valor (atual/ano anterior)</t>
         </is>
       </c>
       <c r="C25" t="n">

</xml_diff>

<commit_message>
g2.3 e g2.4 - adição de categoria com valore fixos para ser usado no bi
</commit_message>
<xml_diff>
--- a/Data/g2.3.xlsx
+++ b/Data/g2.3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,10 +441,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Período</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Categoria</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Valor</t>
         </is>
@@ -458,11 +463,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Quantidade (atual/dez anos antes)</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>69.07756813417191</v>
+          <t>Quantidade 2024/2014</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>67.40443935635693</v>
       </c>
     </row>
     <row r="3">
@@ -473,11 +483,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Quantidade (atual/dez anos antes)</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>51.02146541432979</v>
+          <t>Quantidade 2024/2014</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>68.53318765364655</v>
       </c>
     </row>
     <row r="4">
@@ -488,11 +503,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Quantidade (atual/dez anos antes)</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>-19.79246840347153</v>
+          <t>Quantidade 2024/2014</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>-9.350826619328432</v>
       </c>
     </row>
     <row r="5">
@@ -503,11 +523,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Quantidade (atual/dez anos antes)</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>-61.70297632359825</v>
+          <t>Quantidade 2024/2014</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>-59.33206703373326</v>
       </c>
     </row>
     <row r="6">
@@ -518,11 +543,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Quantidade (atual/dez anos antes)</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>-70.15466408893185</v>
+          <t>Quantidade 2024/2014</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>637.4722838137473</v>
       </c>
     </row>
     <row r="7">
@@ -533,11 +563,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Quantidade (atual/dez anos antes)</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>110.3235747303544</v>
+          <t>Quantidade 2024/2014</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>212.9210042865891</v>
       </c>
     </row>
     <row r="8">
@@ -548,11 +583,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Valor (atual/dez anos antes)</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>39.20704066561322</v>
+          <t>Valor 2024/2014</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>119.0594447084194</v>
       </c>
     </row>
     <row r="9">
@@ -563,11 +603,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Valor (atual/dez anos antes)</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>111.3766687945756</v>
+          <t>Valor 2024/2014</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>42.53980162572068</v>
       </c>
     </row>
     <row r="10">
@@ -578,11 +623,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Valor (atual/dez anos antes)</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>-38.80258191846784</v>
+          <t>Valor 2024/2014</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>-20.88500066046327</v>
       </c>
     </row>
     <row r="11">
@@ -593,11 +643,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Valor (atual/dez anos antes)</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>-75.00701801464335</v>
+          <t>Valor 2024/2014</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>-52.33362673955766</v>
       </c>
     </row>
     <row r="12">
@@ -608,11 +663,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Valor (atual/dez anos antes)</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>-66.55807726662741</v>
+          <t>Valor 2024/2014</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>661.7192065911167</v>
       </c>
     </row>
     <row r="13">
@@ -623,11 +683,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Valor (atual/dez anos antes)</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>33.87882696012225</v>
+          <t>Valor 2024/2014</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Variação em dez anos</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>76.15988489401225</v>
       </c>
     </row>
     <row r="14">
@@ -638,11 +703,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Quantidade (atual/ano anterior)</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>1.850097872071731</v>
+          <t>Quantidade 2024/2023</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>-18.40979541227526</v>
       </c>
     </row>
     <row r="15">
@@ -653,11 +723,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Quantidade (atual/ano anterior)</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>3.885901984784865</v>
+          <t>Quantidade 2024/2023</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1.224477620844457</v>
       </c>
     </row>
     <row r="16">
@@ -668,11 +743,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Quantidade (atual/ano anterior)</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>13.4046328339834</v>
+          <t>Quantidade 2024/2023</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>11.20181579898588</v>
       </c>
     </row>
     <row r="17">
@@ -683,11 +763,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Quantidade (atual/ano anterior)</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>5.811568352656389</v>
+          <t>Quantidade 2024/2023</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1.829587665484669</v>
       </c>
     </row>
     <row r="18">
@@ -698,11 +783,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Quantidade (atual/ano anterior)</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>12.3237835379718</v>
+          <t>Quantidade 2024/2023</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>34.65587044534413</v>
       </c>
     </row>
     <row r="19">
@@ -713,11 +803,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Quantidade (atual/ano anterior)</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>-36.95150115473441</v>
+          <t>Quantidade 2024/2023</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>-6.41025641025641</v>
       </c>
     </row>
     <row r="20">
@@ -728,11 +823,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Valor (atual/ano anterior)</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>38.13303529810645</v>
+          <t>Valor 2024/2023</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>2.934781326149883</v>
       </c>
     </row>
     <row r="21">
@@ -743,11 +843,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Valor (atual/ano anterior)</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>46.60236769419782</v>
+          <t>Valor 2024/2023</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>-36.31319223224396</v>
       </c>
     </row>
     <row r="22">
@@ -758,11 +863,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Valor (atual/ano anterior)</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>32.00053638077491</v>
+          <t>Valor 2024/2023</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>21.18909609656381</v>
       </c>
     </row>
     <row r="23">
@@ -773,11 +883,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Valor (atual/ano anterior)</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>21.47332385208742</v>
+          <t>Valor 2024/2023</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>4.073232865106783</v>
       </c>
     </row>
     <row r="24">
@@ -788,11 +903,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Valor (atual/ano anterior)</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>64.6428865948227</v>
+          <t>Valor 2024/2023</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>38.51361536014834</v>
       </c>
     </row>
     <row r="25">
@@ -803,11 +923,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Valor (atual/ano anterior)</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>-30.40227332240353</v>
+          <t>Valor 2024/2023</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Variação do último ano</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>-7.859334322257486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
g2.3 - atualizado ano mínimo; antes era ano máximo - 10, mas isso gerava 11 anos; então foi corrigido para - 9
</commit_message>
<xml_diff>
--- a/Data/g2.3.xlsx
+++ b/Data/g2.3.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Quantidade 2024/2014</t>
+          <t>Quantidade 2024/2015</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>67.40443935635693</v>
+        <v>42.03766661270304</v>
       </c>
     </row>
     <row r="3">
@@ -483,7 +483,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Quantidade 2024/2014</t>
+          <t>Quantidade 2024/2015</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>68.53318765364655</v>
+        <v>84.08918303135511</v>
       </c>
     </row>
     <row r="4">
@@ -503,7 +503,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Quantidade 2024/2014</t>
+          <t>Quantidade 2024/2015</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>-9.350826619328432</v>
+        <v>-14.5014850570501</v>
       </c>
     </row>
     <row r="5">
@@ -523,7 +523,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Quantidade 2024/2014</t>
+          <t>Quantidade 2024/2015</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>-59.33206703373326</v>
+        <v>-55.51025561441625</v>
       </c>
     </row>
     <row r="6">
@@ -543,7 +543,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Quantidade 2024/2014</t>
+          <t>Quantidade 2024/2015</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>637.4722838137473</v>
+        <v>254.5842217484009</v>
       </c>
     </row>
     <row r="7">
@@ -563,7 +563,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Quantidade 2024/2014</t>
+          <t>Quantidade 2024/2015</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>212.9210042865891</v>
+        <v>301.0989010989011</v>
       </c>
     </row>
     <row r="8">
@@ -583,7 +583,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Valor 2024/2014</t>
+          <t>Valor 2024/2015</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>119.0594447084194</v>
+        <v>70.77527442490312</v>
       </c>
     </row>
     <row r="9">
@@ -603,7 +603,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Valor 2024/2014</t>
+          <t>Valor 2024/2015</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>42.53980162572068</v>
+        <v>44.24612788095496</v>
       </c>
     </row>
     <row r="10">
@@ -623,7 +623,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Valor 2024/2014</t>
+          <t>Valor 2024/2015</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-20.88500066046327</v>
+        <v>-22.80201896534912</v>
       </c>
     </row>
     <row r="11">
@@ -643,7 +643,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Valor 2024/2014</t>
+          <t>Valor 2024/2015</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>-52.33362673955766</v>
+        <v>-52.00431130021104</v>
       </c>
     </row>
     <row r="12">
@@ -663,7 +663,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Valor 2024/2014</t>
+          <t>Valor 2024/2015</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>661.7192065911167</v>
+        <v>311.1692808246118</v>
       </c>
     </row>
     <row r="13">
@@ -683,7 +683,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Valor 2024/2014</t>
+          <t>Valor 2024/2015</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>76.15988489401225</v>
+        <v>96.32603784185962</v>
       </c>
     </row>
     <row r="14">

</xml_diff>

<commit_message>
g2.3 - atualização da estrutura da tabela, conforme solicitado por wagner
</commit_message>
<xml_diff>
--- a/Data/g2.3.xlsx
+++ b/Data/g2.3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,15 +441,10 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Período</t>
+          <t>Variação</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Categoria</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Valor</t>
         </is>
@@ -466,12 +461,7 @@
           <t>Quantidade 2024/2015</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+      <c r="C2" t="n">
         <v>42.03766661270304</v>
       </c>
     </row>
@@ -486,12 +476,7 @@
           <t>Quantidade 2024/2015</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
+      <c r="C3" t="n">
         <v>84.08918303135511</v>
       </c>
     </row>
@@ -506,12 +491,7 @@
           <t>Quantidade 2024/2015</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4" t="n">
         <v>-14.5014850570501</v>
       </c>
     </row>
@@ -526,12 +506,7 @@
           <t>Quantidade 2024/2015</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
+      <c r="C5" t="n">
         <v>-55.51025561441625</v>
       </c>
     </row>
@@ -546,12 +521,7 @@
           <t>Quantidade 2024/2015</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
+      <c r="C6" t="n">
         <v>254.5842217484009</v>
       </c>
     </row>
@@ -566,12 +536,7 @@
           <t>Quantidade 2024/2015</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
+      <c r="C7" t="n">
         <v>301.0989010989011</v>
       </c>
     </row>
@@ -586,12 +551,7 @@
           <t>Valor 2024/2015</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
+      <c r="C8" t="n">
         <v>70.77527442490312</v>
       </c>
     </row>
@@ -606,12 +566,7 @@
           <t>Valor 2024/2015</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
+      <c r="C9" t="n">
         <v>44.24612788095496</v>
       </c>
     </row>
@@ -626,12 +581,7 @@
           <t>Valor 2024/2015</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
+      <c r="C10" t="n">
         <v>-22.80201896534912</v>
       </c>
     </row>
@@ -646,12 +596,7 @@
           <t>Valor 2024/2015</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
+      <c r="C11" t="n">
         <v>-52.00431130021104</v>
       </c>
     </row>
@@ -666,12 +611,7 @@
           <t>Valor 2024/2015</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
+      <c r="C12" t="n">
         <v>311.1692808246118</v>
       </c>
     </row>
@@ -686,12 +626,7 @@
           <t>Valor 2024/2015</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Variação em dez anos</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
+      <c r="C13" t="n">
         <v>96.32603784185962</v>
       </c>
     </row>
@@ -706,12 +641,7 @@
           <t>Quantidade 2024/2023</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
+      <c r="C14" t="n">
         <v>-18.40979541227526</v>
       </c>
     </row>
@@ -726,12 +656,7 @@
           <t>Quantidade 2024/2023</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
+      <c r="C15" t="n">
         <v>1.224477620844457</v>
       </c>
     </row>
@@ -746,12 +671,7 @@
           <t>Quantidade 2024/2023</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
+      <c r="C16" t="n">
         <v>11.20181579898588</v>
       </c>
     </row>
@@ -766,12 +686,7 @@
           <t>Quantidade 2024/2023</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
+      <c r="C17" t="n">
         <v>1.829587665484669</v>
       </c>
     </row>
@@ -786,12 +701,7 @@
           <t>Quantidade 2024/2023</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
+      <c r="C18" t="n">
         <v>34.65587044534413</v>
       </c>
     </row>
@@ -806,12 +716,7 @@
           <t>Quantidade 2024/2023</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
+      <c r="C19" t="n">
         <v>-6.41025641025641</v>
       </c>
     </row>
@@ -826,12 +731,7 @@
           <t>Valor 2024/2023</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
+      <c r="C20" t="n">
         <v>2.934781326149883</v>
       </c>
     </row>
@@ -846,12 +746,7 @@
           <t>Valor 2024/2023</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
+      <c r="C21" t="n">
         <v>-36.31319223224396</v>
       </c>
     </row>
@@ -866,12 +761,7 @@
           <t>Valor 2024/2023</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
+      <c r="C22" t="n">
         <v>21.18909609656381</v>
       </c>
     </row>
@@ -886,12 +776,7 @@
           <t>Valor 2024/2023</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
+      <c r="C23" t="n">
         <v>4.073232865106783</v>
       </c>
     </row>
@@ -906,12 +791,7 @@
           <t>Valor 2024/2023</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
+      <c r="C24" t="n">
         <v>38.51361536014834</v>
       </c>
     </row>
@@ -926,12 +806,7 @@
           <t>Valor 2024/2023</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Variação do último ano</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
+      <c r="C25" t="n">
         <v>-7.859334322257486</v>
       </c>
     </row>

</xml_diff>